<commit_message>
milestone 5 file dump
</commit_message>
<xml_diff>
--- a/Documentation/Asset List.xlsx
+++ b/Documentation/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373A527C-1C6B-4702-A047-A3098FE99F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F1B139-3BCD-4189-9A36-60D42FD61D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -181,13 +181,28 @@
     <t>metal collision</t>
   </si>
   <si>
-    <t>https://freesound.org/people/launemax/sounds/274768/</t>
-  </si>
-  <si>
     <t>https://freesound.org/people/phoenixdk/sounds/80407/</t>
   </si>
   <si>
     <t>whoosh</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Gammelsmurfen778/sounds/474007/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/JohnsonBrandEditing/sounds/173944/</t>
+  </si>
+  <si>
+    <t>shriek (upon death)</t>
+  </si>
+  <si>
+    <t>Victory bells</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/loopsamples.club/sounds/483383/</t>
+  </si>
+  <si>
+    <t>The player collects bells to win, so the victory chime is the sound of several bells.</t>
   </si>
 </sst>
 </file>
@@ -499,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -604,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>47</v>
@@ -624,7 +639,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
@@ -811,6 +826,9 @@
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D20" t="s">
         <v>50</v>
       </c>
@@ -822,11 +840,39 @@
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D21" t="s">
-        <v>52</v>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -836,6 +882,7 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="D17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{65BA944D-A6C0-4ED2-A641-FEFF1A2A72B7}"/>
+    <hyperlink ref="D21" r:id="rId6" xr:uid="{3B04602D-25EA-42E7-B473-A0ED3184A434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>